<commit_message>
Added setupconfig method and began solving bugs in csv read
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpisano/Documents/MAC/Mines/CSCI306/Workspace/ClueGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74E44FB-5A70-FB41-B3B0-BCBFEF66DF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720E0DD-A090-9C48-80C2-4DF05768E58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17360" activeTab="1" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="38">
   <si>
     <t>X</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>&lt;W</t>
   </si>
   <si>
     <t>W&lt;</t>
@@ -216,7 +213,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="36">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -334,6 +331,126 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -798,7 +915,7 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AI9" sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2:AA30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -977,7 +1094,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -1010,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s">
         <v>15</v>
@@ -1040,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z3" t="s">
         <v>3</v>
@@ -1063,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1090,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s">
@@ -1109,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V4" t="s">
         <v>3</v>
@@ -1118,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>3</v>
@@ -1159,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
@@ -1390,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -1423,10 +1540,10 @@
         <v>1</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q8" t="s">
         <v>1</v>
@@ -1450,7 +1567,7 @@
         <v>7</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y8" t="s">
         <v>7</v>
@@ -1521,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U9" t="s">
         <v>7</v>
@@ -1530,7 +1647,7 @@
         <v>7</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>7</v>
@@ -1565,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
         <v>1</v>
@@ -1725,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
@@ -1776,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W12" t="s">
         <v>1</v>
@@ -1808,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>2</v>
@@ -1945,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X14" t="s">
         <v>1</v>
@@ -2063,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
         <v>1</v>
@@ -2229,47 +2346,47 @@
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>0</v>
-      </c>
-      <c r="R18" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" t="s">
-        <v>1</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="U18" t="s">
         <v>12</v>
       </c>
@@ -2280,7 +2397,7 @@
         <v>12</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y18" t="s">
         <v>12</v>
@@ -2363,7 +2480,7 @@
         <v>12</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y19" s="2" t="s">
         <v>12</v>
@@ -2404,7 +2521,7 @@
         <v>6</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
         <v>1</v>
@@ -2472,7 +2589,7 @@
         <v>6</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>6</v>
@@ -2555,7 +2672,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -2668,10 +2785,10 @@
         <v>1</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q23" t="s">
         <v>1</v>
@@ -2695,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="X23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y23" t="s">
         <v>1</v>
@@ -2967,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -2985,7 +3102,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K27" t="s">
         <v>14</v>
@@ -3003,7 +3120,7 @@
         <v>14</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q27" t="s">
         <v>14</v>
@@ -3047,7 +3164,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>5</v>
@@ -3083,7 +3200,7 @@
         <v>14</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>14</v>
@@ -3290,42 +3407,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"J"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:AA30">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"J"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3338,8 +3455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532EE0A-5E4E-0940-A5AF-27E2B28A0057}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3432,7 +3549,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -3465,7 +3582,7 @@
         <v>15</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O2" t="s">
         <v>15</v>
@@ -3495,7 +3612,7 @@
         <v>3</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y2" t="s">
         <v>3</v>
@@ -3515,7 +3632,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -3542,7 +3659,7 @@
         <v>15</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s">
@@ -3561,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U3" t="s">
         <v>3</v>
@@ -3570,7 +3687,7 @@
         <v>3</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>3</v>
@@ -3608,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -3830,7 +3947,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -3863,10 +3980,10 @@
         <v>1</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
         <v>1</v>
@@ -3890,7 +4007,7 @@
         <v>7</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X7" t="s">
         <v>7</v>
@@ -3958,7 +4075,7 @@
         <v>1</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T8" t="s">
         <v>7</v>
@@ -3967,7 +4084,7 @@
         <v>7</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>7</v>
@@ -3999,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
@@ -4153,7 +4270,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -4204,7 +4321,7 @@
         <v>1</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V11" t="s">
         <v>1</v>
@@ -4233,7 +4350,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
@@ -4367,7 +4484,7 @@
         <v>1</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W13" t="s">
         <v>1</v>
@@ -4479,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
         <v>1</v>
@@ -4639,47 +4756,47 @@
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="T17" t="s">
         <v>12</v>
       </c>
@@ -4690,7 +4807,7 @@
         <v>12</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X17" t="s">
         <v>12</v>
@@ -4770,7 +4887,7 @@
         <v>12</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>12</v>
@@ -4808,7 +4925,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
         <v>1</v>
@@ -4873,7 +4990,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>6</v>
@@ -4953,7 +5070,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -5063,10 +5180,10 @@
         <v>1</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P22" t="s">
         <v>1</v>
@@ -5090,7 +5207,7 @@
         <v>1</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X22" t="s">
         <v>1</v>
@@ -5350,7 +5467,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -5368,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J26" t="s">
         <v>14</v>
@@ -5386,7 +5503,7 @@
         <v>14</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P26" t="s">
         <v>14</v>
@@ -5427,7 +5544,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -5463,7 +5580,7 @@
         <v>14</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>14</v>
@@ -5663,7 +5780,39 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A30:XFD1048576 AA1:XFD29">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>"L"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
+      <formula>"H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+      <formula>"J"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Z29">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"W"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added blank methods so code compiles with 306 test still has many errors
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpisano/Documents/MAC/Mines/CSCI306/Workspace/ClueGame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720E0DD-A090-9C48-80C2-4DF05768E58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B0E203-1D67-824B-A2B9-B09853F1D211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17360" activeTab="1" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17360" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="CSV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -213,127 +213,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -914,11 +794,14 @@
   </sheetPr>
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AA30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="29" max="29" width="63.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -3407,42 +3290,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"J"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:AA30">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"J"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3455,8 +3338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532EE0A-5E4E-0940-A5AF-27E2B28A0057}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Z29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4813,7 +4696,7 @@
         <v>12</v>
       </c>
       <c r="Y17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z17" t="s">
         <v>12</v>
@@ -5780,76 +5663,44 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A30:XFD1048576 AA1:XFD29">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+  <conditionalFormatting sqref="A1:Z29">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"J"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"J"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z29">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>"W"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
-      <formula>"L"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"C"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
-      <formula>"J"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z29">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
-      <formula>"J"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
-      <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feature: Added missing character in the sheet
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpisano/Documents/MAC/Mines/CSCI306/Workspace/ClueGame/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klduf\Desktop\Clue Game\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B0E203-1D67-824B-A2B9-B09853F1D211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF02E372-ABD5-46B4-96B1-C8E5F95CC278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17360" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="38">
   <si>
     <t>X</t>
   </si>
@@ -795,15 +795,15 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.296875" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="29" max="29" width="63.33203125" customWidth="1"/>
+    <col min="29" max="29" width="63.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -883,7 +883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -966,7 +966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1092,7 +1092,9 @@
       <c r="N4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="P4" t="s">
         <v>15</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1213,7 +1215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1462,7 +1464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1545,7 +1547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1711,7 +1713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1794,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1960,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2043,7 +2045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2126,7 +2128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2209,7 +2211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2292,7 +2294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2375,7 +2377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2458,7 +2460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2624,7 +2626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2707,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2790,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2873,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2956,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3039,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3122,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3205,7 +3207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3342,9 +3344,9 @@
       <selection activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.296875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3424,7 +3426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3504,7 +3506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3582,7 +3584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -3982,7 +3984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4062,7 +4064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -4142,7 +4144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -4222,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -4382,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -4462,7 +4464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4542,7 +4544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -4622,7 +4624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -4702,7 +4704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -4782,7 +4784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -4862,7 +4864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -4942,7 +4944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -5022,7 +5024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -5102,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -5182,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -5262,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -5342,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -5422,7 +5424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -5502,7 +5504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -5582,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>5</v>
       </c>

</xml_diff>